<commit_message>
fix: changes in solutions
</commit_message>
<xml_diff>
--- a/lab3/real_estate_krym_filtered.xlsx
+++ b/lab3/real_estate_krym_filtered.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,20 +468,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10063648</t>
+          <t>10132208</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1-к, ул.Шевченко д-16, 5-й микрорайон.</t>
+          <t>Сдаются в аренду места для бровиста/визажиста</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>35000</v>
+        <v>11000</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Сегодня, 01:22</t>
+          <t>Сегодня, 15:31</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,27 +491,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 45; Этаж: 4; Этажей в доме: 6;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Салон красоты; Готовый бизнес: нет;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7636563</t>
+          <t>9990054</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1-к квартира, Степаняна-15, 36 м2, 1/5 эт.</t>
+          <t>1-к, Дмитрия Ульянова-2, Стрелецкая бухта, Гагаринский район.</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>27000</v>
+        <v>25000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Сегодня, 01:18</t>
+          <t>Сегодня, 13:35</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -521,27 +521,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 36; Этаж: 1; Этажей в доме: 5;</t>
+          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 36; Этаж: 3; Этажей в доме: 5;</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8120158</t>
+          <t>8652548</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1-к квартира, Парковая-11, 45 м2, 6/10 эт.</t>
+          <t>1-к квартира, Дмитрия Ульянова-2, 36 м2, 3/5 эт.</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>40000</v>
+        <v>25000</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Сегодня, 01:18</t>
+          <t>Сегодня, 13:35</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,458 +551,277 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Монолитный; Площадь: 45; Этаж: 6; Этажей в доме: 10;</t>
+          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 36; Этаж: 3; Этажей в доме: 5;</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>9973018</t>
+          <t>10132004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1-к, ПОР-89, Лётчики, Гагаринский район.</t>
+          <t>Арендуй выгодно офис в Евпатории</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>27000</v>
+        <v>10000</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Сегодня, 01:17</t>
+          <t>Сегодня, 13:25</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Евпатория</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 34; Этаж: 4; Этажей в доме: 5;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Офис; Готовый бизнес: нет;</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>9794766</t>
+          <t>5307964</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1-к, Античный-20 А, Омега, Гагаринский район.</t>
+          <t>Сдам нежилое помещение</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>38000</v>
+        <v>25000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Сегодня, 01:17</t>
+          <t>Сегодня, 08:47</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Монолитный; Площадь: 50; Этаж: 6; Этажей в доме: 10;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Помещение; Готовый бизнес: нет;</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10097584</t>
+          <t>7105101</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2-к квартира, ПОР-40, Лётчики. 58 м2, 3/9 эт.</t>
+          <t>Сдам нежилое помещение.</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>30000</v>
+        <v>23000</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Сегодня, 01:16</t>
+          <t>Сегодня, 08:47</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 2; Тип дома: Панельный; Площадь: 58; Этаж: 3; Этажей в доме: 9;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Помещение; Готовый бизнес: да;</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10106903</t>
+          <t>1864998</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1-к квартира, ул.Челнокова д-12/3, Омега. 44 м2, 5/5 эт.</t>
+          <t>Аренда магазина в Крыму на берегу Черного моря.</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Сегодня, 01:16</t>
+          <t>Сегодня, 08:01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 44; Этаж: 5; Этажей в доме: 5;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Магазин; Готовый бизнес: да;</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>10104223</t>
+          <t>10096859</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1-к, Гайдара-5, Стрелецкая бухта, Гагаринский район.</t>
+          <t>Аренда 2 х комнатной квартиры Симферопольский район село Мирное</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Сегодня, 01:16</t>
+          <t>Сегодня, 06:09</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Тип дома: Блочный; Площадь: 36; Этаж: 1; Этажей в доме: 5;</t>
+          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 2; Площадь: 46; Этаж: 1; Этажей в доме: 1;</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>10106617</t>
+          <t>10052833</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2-к, пр-т Октябрьской Революции д-40, Лётчики. 58 м2, 3/9 эт.</t>
+          <t>Аренда складского помещение ул Индустриальная /ул Лексина</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>30000</v>
+        <v>36000</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Сегодня, 01:15</t>
+          <t>Сегодня, 06:08</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 2; Тип дома: Панельный; Площадь: 58; Этаж: 3; Этажей в доме: 9;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Склад;</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10107999</t>
+          <t>9677392</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Однокомнатная на Хрусталёва. 23 000</t>
+          <t>Аренда помещение свободного назначение</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>23000</v>
+        <v>30000</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Вчера, 22:40</t>
+          <t>Сегодня, 06:06</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Площадь: 40; Этаж: 4; Этажей в доме: 5;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Салон красоты;</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10090609</t>
+          <t>9150844</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Однокомнатная на Колобова, 22. 27 000</t>
+          <t>Аренда торгового помещение</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Вчера, 22:40</t>
+          <t>Сегодня, 06:05</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Севастополь</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Срок аренды: На длительный срок; Количество комнат: 1; Площадь: 42; Этаж: 3; Этажей в доме: 10;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Магазин; Готовый бизнес: да;</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4069805</t>
+          <t>5847411</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Солидное помещение для серьёзных товарищей!</t>
+          <t>Аренда помещение свободного назначение</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>39000</v>
+        <v>40000</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Вчера, 21:08</t>
+          <t>Сегодня, 06:03</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Евпатория</t>
+          <t>Симферополь</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Тип объявления: Сдам; Вид объекта: Помещение;</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>10109199</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Сдaется многоцeлевoе помещение пoд офиc, салон, склaд, магазин и т.д.</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>20000</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Вчера, 14:44</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам;</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>10109150</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Сдается трехкомнатный одноэтажный дом на ул. Полоцкая в районе Горпищенко.</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Вчера, 14:44</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам;</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>10109151</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1-к квартира, 30 м2, 1/1 эт.</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>20000</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Вчера, 14:44</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам; Количество комнат: 1; Тип дома: Блочный; Площадь: 30; Этаж: 1; Этажей в доме: 1;</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>10109088</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1-к квартира, 40 м2, 2/5 эт.</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>45000</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Вчера, 14:44</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам; Количество комнат: 1; Тип дома: Блочный; Площадь: 40; Этаж: 2; Этажей в доме: 5;</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>10109043</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2-к квартира, 63 м2, 3/9 эт.</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Вчера, 14:43</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам; Количество комнат: 2; Тип дома: Монолитный; Площадь: 63; Этаж: 3; Этажей в доме: 9;</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>10109035</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Объект № 75740
-Сдам на длительный срок дом на Северной стороне рядом с парком</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>22000</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Вчера, 14:43</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Севастополь</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Тип объявления: Сдам;</t>
+          <t>Тип объявления: Сдам; Вид объекта: Помещение; Готовый бизнес: да;</t>
         </is>
       </c>
     </row>

</xml_diff>